<commit_message>
#fixed the dungeon stuff
</commit_message>
<xml_diff>
--- a/Senior Project Files/Wbs Who.xlsx
+++ b/Senior Project Files/Wbs Who.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="21015" windowHeight="9975"/>
+    <workbookView xWindow="360" yWindow="45" windowWidth="19440" windowHeight="9975"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="72">
   <si>
     <t>Task</t>
   </si>
@@ -189,9 +189,6 @@
     <t>Alex</t>
   </si>
   <si>
-    <t>Alex, Matt</t>
-  </si>
-  <si>
     <t>Art</t>
   </si>
   <si>
@@ -205,6 +202,36 @@
   </si>
   <si>
     <t>Alex, Outside Source</t>
+  </si>
+  <si>
+    <t>Bosses</t>
+  </si>
+  <si>
+    <t>NPC</t>
+  </si>
+  <si>
+    <t>Goal***!*!*!*!*!*!*!*!*!**!!!</t>
+  </si>
+  <si>
+    <t>Adding Content</t>
+  </si>
+  <si>
+    <t>Alex*, John, Matt</t>
+  </si>
+  <si>
+    <t>Alex*, John</t>
+  </si>
+  <si>
+    <t>Alex, John, Matt*</t>
+  </si>
+  <si>
+    <t>John*, Matt</t>
+  </si>
+  <si>
+    <t>Alex, John*, Joe</t>
+  </si>
+  <si>
+    <t>Alex*, Matt</t>
   </si>
 </sst>
 </file>
@@ -536,10 +563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -563,24 +590,24 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
         <v>61</v>
-      </c>
-      <c r="B2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" t="s">
         <v>58</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>59</v>
-      </c>
-      <c r="C3" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -613,7 +640,7 @@
         <v>45</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -624,7 +651,7 @@
         <v>45</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -668,7 +695,7 @@
         <v>45</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -679,7 +706,7 @@
         <v>45</v>
       </c>
       <c r="C12" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -712,7 +739,7 @@
         <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -745,7 +772,7 @@
         <v>46</v>
       </c>
       <c r="C18" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -756,7 +783,7 @@
         <v>46</v>
       </c>
       <c r="C19" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -783,47 +810,62 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="B22" t="s">
         <v>48</v>
+      </c>
+      <c r="C22" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="B23" t="s">
-        <v>48</v>
+        <v>46</v>
+      </c>
+      <c r="C23" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="B24" t="s">
-        <v>48</v>
+        <v>46</v>
+      </c>
+      <c r="C24" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B25" t="s">
         <v>48</v>
+      </c>
+      <c r="C25" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B26" t="s">
         <v>48</v>
+      </c>
+      <c r="C26" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B27" t="s">
         <v>48</v>
@@ -831,7 +873,7 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B28" t="s">
         <v>48</v>
@@ -839,7 +881,7 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B29" t="s">
         <v>48</v>
@@ -847,7 +889,7 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B30" t="s">
         <v>48</v>
@@ -855,7 +897,7 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B31" t="s">
         <v>48</v>
@@ -863,113 +905,152 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>30</v>
+      </c>
+      <c r="B34" t="s">
+        <v>48</v>
+      </c>
+      <c r="C34" t="s">
+        <v>56</v>
+      </c>
+      <c r="D34" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
         <v>31</v>
       </c>
-      <c r="B32" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" t="s">
+      <c r="B35" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
         <v>32</v>
       </c>
-      <c r="B33" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" t="s">
+      <c r="B36" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
         <v>33</v>
       </c>
-      <c r="B34" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" t="s">
+      <c r="B37" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
         <v>34</v>
       </c>
-      <c r="B35" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" t="s">
+      <c r="B38" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
         <v>35</v>
       </c>
-      <c r="B36" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" t="s">
+      <c r="B39" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
         <v>36</v>
       </c>
-      <c r="B37" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38" t="s">
+      <c r="B40" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
         <v>37</v>
       </c>
-      <c r="B38" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
-      <c r="A39" t="s">
+      <c r="B41" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
         <v>38</v>
       </c>
-      <c r="B39" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
-      <c r="A40" t="s">
+      <c r="B42" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
         <v>39</v>
       </c>
-      <c r="B40" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
-      <c r="A41" t="s">
+      <c r="B43" t="s">
+        <v>45</v>
+      </c>
+      <c r="C43" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
         <v>40</v>
       </c>
-      <c r="B41" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
-      <c r="A42" t="s">
+      <c r="B44" t="s">
+        <v>45</v>
+      </c>
+      <c r="C44" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
         <v>41</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B45" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="43" spans="1:2">
-      <c r="A43" t="s">
+      <c r="C45" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
         <v>42</v>
       </c>
-      <c r="B43" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
-      <c r="A44" t="s">
+      <c r="B46" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
         <v>43</v>
       </c>
-      <c r="B44" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
-      <c r="A45" t="s">
+      <c r="B47" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
         <v>44</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B48" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>

<commit_message>
#changed a bunch of the tiles and added a bunch. Also modified the maps to refelct the changes. Updated the wbs a little, and added the key to what each character means in the maps
</commit_message>
<xml_diff>
--- a/Senior Project Files/Wbs Who.xlsx
+++ b/Senior Project Files/Wbs Who.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="45" windowWidth="19440" windowHeight="9975"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="161">
   <si>
     <t>Task</t>
   </si>
@@ -487,13 +487,25 @@
   </si>
   <si>
     <t>On Hold/Late</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>done-late</t>
+  </si>
+  <si>
+    <t>late 1month</t>
+  </si>
+  <si>
+    <t>needs pathfinding</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -534,6 +546,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -612,6 +629,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -646,6 +664,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -821,14 +840,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" customWidth="1"/>
@@ -839,7 +858,7 @@
     <col min="7" max="7" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -862,7 +881,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -871,7 +890,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>59</v>
       </c>
@@ -888,7 +907,7 @@
       </c>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>103</v>
       </c>
@@ -906,7 +925,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>104</v>
       </c>
@@ -926,7 +945,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>56</v>
       </c>
@@ -943,7 +962,7 @@
       </c>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>70</v>
       </c>
@@ -963,7 +982,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>72</v>
       </c>
@@ -983,7 +1002,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>74</v>
       </c>
@@ -1003,7 +1022,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>81</v>
       </c>
@@ -1023,7 +1042,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>116</v>
       </c>
@@ -1044,7 +1063,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>3</v>
       </c>
@@ -1065,7 +1084,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
@@ -1086,7 +1105,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
@@ -1107,7 +1126,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>76</v>
       </c>
@@ -1123,7 +1142,7 @@
       <c r="E15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>77</v>
       </c>
@@ -1139,7 +1158,7 @@
       <c r="E16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>78</v>
       </c>
@@ -1155,7 +1174,7 @@
       <c r="E17" s="1"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
@@ -1178,7 +1197,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>114</v>
       </c>
@@ -1201,7 +1220,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>12</v>
       </c>
@@ -1224,7 +1243,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>7</v>
       </c>
@@ -1247,7 +1266,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -1270,7 +1289,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>8</v>
       </c>
@@ -1293,7 +1312,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>9</v>
       </c>
@@ -1316,7 +1335,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>10</v>
       </c>
@@ -1339,7 +1358,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>11</v>
       </c>
@@ -1362,7 +1381,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>13</v>
       </c>
@@ -1385,7 +1404,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>82</v>
       </c>
@@ -1399,9 +1418,11 @@
         <v>26</v>
       </c>
       <c r="E28" s="1"/>
-      <c r="G28" s="1"/>
-    </row>
-    <row r="29" spans="1:7">
+      <c r="G28" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>83</v>
       </c>
@@ -1415,9 +1436,11 @@
         <v>26</v>
       </c>
       <c r="E29" s="1"/>
-      <c r="G29" s="1"/>
-    </row>
-    <row r="30" spans="1:7">
+      <c r="G29" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>84</v>
       </c>
@@ -1431,9 +1454,11 @@
         <v>26</v>
       </c>
       <c r="E30" s="1"/>
-      <c r="G30" s="1"/>
-    </row>
-    <row r="31" spans="1:7">
+      <c r="G30" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>85</v>
       </c>
@@ -1447,9 +1472,11 @@
         <v>26</v>
       </c>
       <c r="E31" s="1"/>
-      <c r="G31" s="1"/>
-    </row>
-    <row r="32" spans="1:7">
+      <c r="G31" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>14</v>
       </c>
@@ -1472,7 +1499,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>15</v>
       </c>
@@ -1495,7 +1522,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>86</v>
       </c>
@@ -1509,9 +1536,11 @@
         <v>32</v>
       </c>
       <c r="E34" s="1"/>
-      <c r="G34" s="1"/>
-    </row>
-    <row r="35" spans="1:7">
+      <c r="G34" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>87</v>
       </c>
@@ -1525,9 +1554,11 @@
         <v>124</v>
       </c>
       <c r="E35" s="1"/>
-      <c r="G35" s="1"/>
-    </row>
-    <row r="36" spans="1:7">
+      <c r="G35" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>16</v>
       </c>
@@ -1550,7 +1581,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>17</v>
       </c>
@@ -1570,7 +1601,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>88</v>
       </c>
@@ -1584,9 +1615,11 @@
         <v>36</v>
       </c>
       <c r="E38" s="1"/>
-      <c r="G38" s="1"/>
-    </row>
-    <row r="39" spans="1:7">
+      <c r="G38" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>89</v>
       </c>
@@ -1600,9 +1633,11 @@
         <v>126</v>
       </c>
       <c r="E39" s="1"/>
-      <c r="G39" s="1"/>
-    </row>
-    <row r="40" spans="1:7">
+      <c r="G39" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>18</v>
       </c>
@@ -1625,7 +1660,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>90</v>
       </c>
@@ -1639,9 +1674,11 @@
         <v>39</v>
       </c>
       <c r="E41" s="1"/>
-      <c r="G41" s="1"/>
-    </row>
-    <row r="42" spans="1:7">
+      <c r="G41" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>91</v>
       </c>
@@ -1655,9 +1692,11 @@
         <v>39</v>
       </c>
       <c r="E42" s="1"/>
-      <c r="G42" s="1"/>
-    </row>
-    <row r="43" spans="1:7">
+      <c r="G42" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>19</v>
       </c>
@@ -1680,7 +1719,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>92</v>
       </c>
@@ -1694,9 +1733,11 @@
         <v>15</v>
       </c>
       <c r="E44" s="1"/>
-      <c r="G44" s="1"/>
-    </row>
-    <row r="45" spans="1:7">
+      <c r="G44" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>93</v>
       </c>
@@ -1710,9 +1751,11 @@
         <v>15</v>
       </c>
       <c r="E45" s="1"/>
-      <c r="G45" s="1"/>
-    </row>
-    <row r="46" spans="1:7">
+      <c r="G45" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>94</v>
       </c>
@@ -1726,14 +1769,16 @@
         <v>15</v>
       </c>
       <c r="E46" s="1"/>
-      <c r="G46" s="1"/>
-    </row>
-    <row r="47" spans="1:7">
+      <c r="G46" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
       <c r="G47" s="1"/>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>61</v>
       </c>
@@ -1756,7 +1801,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>95</v>
       </c>
@@ -1770,9 +1815,11 @@
         <v>47</v>
       </c>
       <c r="E49" s="1"/>
-      <c r="G49" s="1"/>
-    </row>
-    <row r="50" spans="1:7">
+      <c r="G49" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>96</v>
       </c>
@@ -1786,9 +1833,11 @@
         <v>47</v>
       </c>
       <c r="E50" s="1"/>
-      <c r="G50" s="1"/>
-    </row>
-    <row r="51" spans="1:7">
+      <c r="G50" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>63</v>
       </c>
@@ -1802,9 +1851,11 @@
         <v>129</v>
       </c>
       <c r="E51" s="1"/>
-      <c r="G51" s="1"/>
-    </row>
-    <row r="52" spans="1:7">
+      <c r="G51" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>62</v>
       </c>
@@ -1827,7 +1878,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>21</v>
       </c>
@@ -1850,7 +1901,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>97</v>
       </c>
@@ -1864,9 +1915,11 @@
         <v>14</v>
       </c>
       <c r="E54" s="1"/>
-      <c r="G54" s="1"/>
-    </row>
-    <row r="55" spans="1:7">
+      <c r="G54" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>98</v>
       </c>
@@ -1880,14 +1933,16 @@
         <v>131</v>
       </c>
       <c r="E55" s="1"/>
-      <c r="G55" s="1"/>
-    </row>
-    <row r="56" spans="1:7">
+      <c r="G55" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>53</v>
@@ -1902,10 +1957,10 @@
         <v>40648</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>23</v>
       </c>
@@ -1924,7 +1979,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>24</v>
       </c>
@@ -1945,7 +2000,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>25</v>
       </c>
@@ -1966,7 +2021,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>26</v>
       </c>
@@ -1987,7 +2042,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -1995,7 +2050,7 @@
       <c r="E61" s="1"/>
       <c r="G61" s="1"/>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>27</v>
       </c>
@@ -2014,7 +2069,7 @@
       </c>
       <c r="G62" s="1"/>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>28</v>
       </c>
@@ -2031,7 +2086,7 @@
       </c>
       <c r="G63" s="1"/>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>29</v>
       </c>
@@ -2052,7 +2107,7 @@
       </c>
       <c r="G64" s="1"/>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>30</v>
       </c>
@@ -2071,7 +2126,7 @@
       </c>
       <c r="G65" s="1"/>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>31</v>
       </c>
@@ -2090,7 +2145,7 @@
       </c>
       <c r="G66" s="1"/>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>32</v>
       </c>
@@ -2109,7 +2164,7 @@
       </c>
       <c r="G67" s="1"/>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>33</v>
       </c>
@@ -2128,7 +2183,7 @@
       </c>
       <c r="G68" s="1"/>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>34</v>
       </c>
@@ -2147,7 +2202,7 @@
       </c>
       <c r="G69" s="1"/>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>35</v>
       </c>
@@ -2166,7 +2221,7 @@
       </c>
       <c r="G70" s="1"/>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>36</v>
       </c>
@@ -2185,7 +2240,7 @@
       </c>
       <c r="G71" s="1"/>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>37</v>
       </c>
@@ -2204,7 +2259,7 @@
       </c>
       <c r="G72" s="1"/>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>38</v>
       </c>
@@ -2225,7 +2280,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>39</v>
       </c>
@@ -2246,7 +2301,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>40</v>
       </c>
@@ -2267,7 +2322,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>41</v>
       </c>
@@ -2281,7 +2336,7 @@
       </c>
       <c r="G76" s="1"/>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>42</v>
       </c>
@@ -2295,7 +2350,7 @@
       </c>
       <c r="G77" s="1"/>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>43</v>
       </c>
@@ -2316,24 +2371,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
#World barriers in, bug fixed with dungeons, sound effects in
</commit_message>
<xml_diff>
--- a/Senior Project Files/Wbs Who.xlsx
+++ b/Senior Project Files/Wbs Who.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="166">
   <si>
     <t>Task</t>
   </si>
@@ -499,6 +499,21 @@
   </si>
   <si>
     <t>needs pathfinding</t>
+  </si>
+  <si>
+    <t>Behind- Done</t>
+  </si>
+  <si>
+    <t>Matt/Alex</t>
+  </si>
+  <si>
+    <t>Alex/ Joe</t>
+  </si>
+  <si>
+    <t>Ai - PathFinding</t>
+  </si>
+  <si>
+    <t>Joe</t>
   </si>
 </sst>
 </file>
@@ -841,10 +856,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G78"/>
+  <dimension ref="A1:G79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1586,7 +1601,7 @@
         <v>17</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>66</v>
@@ -1606,7 +1621,7 @@
         <v>88</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>73</v>
@@ -1624,7 +1639,7 @@
         <v>89</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>51</v>
@@ -1642,7 +1657,7 @@
         <v>18</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>69</v>
@@ -1704,7 +1719,7 @@
         <v>45</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>55</v>
+        <v>163</v>
       </c>
       <c r="D43" s="1">
         <v>15</v>
@@ -1721,25 +1736,22 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>92</v>
+        <v>164</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D44" s="1">
-        <v>15</v>
-      </c>
+        <v>165</v>
+      </c>
+      <c r="D44" s="1"/>
       <c r="E44" s="1"/>
-      <c r="G44" s="1" t="s">
-        <v>157</v>
-      </c>
+      <c r="F44" s="2"/>
+      <c r="G44" s="1"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>44</v>
@@ -1752,12 +1764,12 @@
       </c>
       <c r="E45" s="1"/>
       <c r="G45" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>44</v>
@@ -1770,64 +1782,64 @@
       </c>
       <c r="E46" s="1"/>
       <c r="G46" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D47" s="1">
+        <v>15</v>
+      </c>
+      <c r="E47" s="1"/>
+      <c r="G47" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-      <c r="G47" s="1"/>
-    </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F48" s="2">
-        <v>40637</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>148</v>
-      </c>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="G48" s="1"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>95</v>
+        <v>61</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D49" s="1">
-        <v>47</v>
-      </c>
-      <c r="E49" s="1"/>
+        <v>52</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F49" s="2">
+        <v>40637</v>
+      </c>
       <c r="G49" s="1" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D50" s="1">
         <v>47</v>
@@ -1839,71 +1851,66 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>63</v>
+        <v>96</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>129</v>
+        <v>53</v>
+      </c>
+      <c r="D51" s="1">
+        <v>47</v>
       </c>
       <c r="E51" s="1"/>
       <c r="G51" s="1" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F52" s="2">
-        <v>40643</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="E52" s="1"/>
       <c r="G52" s="1" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>50</v>
+        <v>162</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="F53" s="2">
-        <v>40637</v>
+        <v>40643</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>44</v>
@@ -1911,17 +1918,22 @@
       <c r="C54" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D54" s="1">
-        <v>14</v>
-      </c>
-      <c r="E54" s="1"/>
+      <c r="D54" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F54" s="2">
+        <v>40637</v>
+      </c>
       <c r="G54" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>44</v>
@@ -1929,8 +1941,8 @@
       <c r="C55" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D55" s="1" t="s">
-        <v>131</v>
+      <c r="D55" s="1">
+        <v>14</v>
       </c>
       <c r="E55" s="1"/>
       <c r="G55" s="1" t="s">
@@ -1939,57 +1951,56 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>22</v>
+        <v>98</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E56" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="F56" s="2">
-        <v>40648</v>
-      </c>
+      <c r="E56" s="1"/>
       <c r="G56" s="1" t="s">
-        <v>44</v>
+        <v>157</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>131</v>
+      </c>
       <c r="E57" s="1" t="s">
-        <v>106</v>
+        <v>143</v>
       </c>
       <c r="F57" s="2">
         <v>40648</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>155</v>
+        <v>44</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C58" s="1"/>
-      <c r="D58" s="1">
-        <v>55</v>
-      </c>
+      <c r="C58" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D58" s="1"/>
       <c r="E58" s="1" t="s">
         <v>106</v>
       </c>
@@ -2002,17 +2013,19 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C59" s="1"/>
+      <c r="C59" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="D59" s="1">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>137</v>
+        <v>106</v>
       </c>
       <c r="F59" s="2">
         <v>40648</v>
@@ -2023,14 +2036,14 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C60" s="1"/>
       <c r="D60" s="1">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>137</v>
@@ -2043,62 +2056,68 @@
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="1"/>
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
-      <c r="E61" s="1"/>
-      <c r="G61" s="1"/>
+      <c r="A61" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D61" s="1">
+        <v>58</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F61" s="2">
+        <v>40648</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>47</v>
-      </c>
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
       <c r="C62" s="1"/>
-      <c r="D62" s="1">
-        <v>21</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F62" s="2">
-        <v>40661</v>
-      </c>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
       <c r="G62" s="1"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C63" s="1"/>
-      <c r="D63" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D63" s="1">
+        <v>21</v>
+      </c>
       <c r="E63" s="1" t="s">
         <v>142</v>
       </c>
       <c r="F63" s="2">
         <v>40661</v>
       </c>
-      <c r="G63" s="1"/>
+      <c r="G63" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>132</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
       <c r="E64" s="1" t="s">
         <v>142</v>
       </c>
@@ -2109,36 +2128,40 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C65" s="1"/>
-      <c r="D65" s="1">
-        <v>36</v>
+        <v>44</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>132</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="F65" s="2">
-        <v>40679</v>
+        <v>40661</v>
       </c>
       <c r="G65" s="1"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C66" s="1"/>
-      <c r="D66" s="1" t="s">
-        <v>133</v>
+      <c r="C66" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D66" s="1">
+        <v>36</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="F66" s="2">
         <v>40679</v>
@@ -2147,17 +2170,17 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C67" s="1"/>
-      <c r="D67" s="1">
-        <v>61</v>
+      <c r="D67" s="1" t="s">
+        <v>133</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="F67" s="2">
         <v>40679</v>
@@ -2166,14 +2189,14 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C68" s="1"/>
-      <c r="D68" s="1" t="s">
-        <v>134</v>
+      <c r="D68" s="1">
+        <v>61</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>137</v>
@@ -2185,17 +2208,17 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C69" s="1"/>
-      <c r="D69" s="1">
-        <v>63</v>
+      <c r="D69" s="1" t="s">
+        <v>134</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>106</v>
+        <v>137</v>
       </c>
       <c r="F69" s="2">
         <v>40679</v>
@@ -2204,36 +2227,36 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C70" s="1"/>
       <c r="D70" s="1">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>142</v>
+        <v>106</v>
       </c>
       <c r="F70" s="2">
-        <v>40688</v>
+        <v>40679</v>
       </c>
       <c r="G70" s="1"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C71" s="1"/>
-      <c r="D71" s="1" t="s">
-        <v>135</v>
+      <c r="D71" s="1">
+        <v>51</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="F71" s="2">
         <v>40688</v>
@@ -2242,47 +2265,45 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C72" s="1"/>
       <c r="D72" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="F72" s="2">
-        <v>40695</v>
+        <v>40688</v>
       </c>
       <c r="G72" s="1"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D73" s="1"/>
+        <v>47</v>
+      </c>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1" t="s">
+        <v>136</v>
+      </c>
       <c r="E73" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F73" s="2">
-        <v>40618</v>
-      </c>
-      <c r="G73" s="1" t="s">
-        <v>152</v>
-      </c>
+        <v>40695</v>
+      </c>
+      <c r="G73" s="1"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>44</v>
@@ -2292,53 +2313,60 @@
       </c>
       <c r="D74" s="1"/>
       <c r="E74" s="1" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="F74" s="2">
-        <v>40623</v>
+        <v>40618</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>107</v>
+        <v>152</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>55</v>
       </c>
       <c r="D75" s="1"/>
       <c r="E75" s="1" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="F75" s="2">
-        <v>40644</v>
+        <v>40623</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>156</v>
+        <v>107</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C76" s="1"/>
+        <v>48</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="D76" s="1"/>
       <c r="E76" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="G76" s="1"/>
+      <c r="F76" s="2">
+        <v>40644</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>47</v>
@@ -2346,13 +2374,13 @@
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
       <c r="E77" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="G77" s="1"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>47</v>
@@ -2360,9 +2388,23 @@
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
       <c r="E78" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G78" s="1"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C79" s="1"/>
+      <c r="D79" s="1"/>
+      <c r="E79" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="G78" s="1"/>
+      <c r="G79" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
#other sprites are here, Also other stuff
</commit_message>
<xml_diff>
--- a/Senior Project Files/Wbs Who.xlsx
+++ b/Senior Project Files/Wbs Who.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="165">
   <si>
     <t>Task</t>
   </si>
@@ -154,9 +154,6 @@
   </si>
   <si>
     <t>Started</t>
-  </si>
-  <si>
-    <t>Not Implemented</t>
   </si>
   <si>
     <t>Not Started</t>
@@ -858,8 +855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -884,16 +881,16 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -907,13 +904,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -924,51 +921,51 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D5" s="1">
         <v>3</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -979,103 +976,103 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="C7" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="D8" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="C9" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F11" s="2">
         <v>40605</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1086,17 +1083,17 @@
         <v>44</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F12" s="2">
         <v>40605</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1107,17 +1104,17 @@
         <v>44</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F13" s="2">
         <v>40605</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1128,63 +1125,63 @@
         <v>44</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F14" s="2">
         <v>40605</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E15" s="1"/>
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E16" s="1"/>
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="D17" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E17" s="1"/>
       <c r="G17" s="1"/>
@@ -1194,45 +1191,45 @@
         <v>6</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F18" s="2">
         <v>40611</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D19" s="1">
         <v>13</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F19" s="2">
         <v>40605</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1243,19 +1240,19 @@
         <v>44</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F20" s="2">
         <v>40611</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1266,19 +1263,19 @@
         <v>44</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F21" s="2">
         <v>40611</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1289,19 +1286,19 @@
         <v>45</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F22" s="2">
         <v>40637</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1312,19 +1309,19 @@
         <v>44</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D23" s="1">
         <v>14</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F23" s="2">
         <v>40618</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1335,19 +1332,19 @@
         <v>44</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D24" s="1">
         <v>13</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F24" s="2">
         <v>40618</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1358,19 +1355,19 @@
         <v>44</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F25" s="2">
         <v>40618</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1381,19 +1378,19 @@
         <v>44</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F26" s="2">
         <v>40618</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1404,91 +1401,91 @@
         <v>45</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D27" s="1">
         <v>18</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F27" s="2">
         <v>40626</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D28" s="1">
         <v>26</v>
       </c>
       <c r="E28" s="1"/>
       <c r="G28" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D29" s="1">
         <v>26</v>
       </c>
       <c r="E29" s="1"/>
       <c r="G29" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D30" s="1">
         <v>26</v>
       </c>
       <c r="E30" s="1"/>
       <c r="G30" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D31" s="1">
         <v>26</v>
       </c>
       <c r="E31" s="1"/>
       <c r="G31" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1499,19 +1496,19 @@
         <v>44</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F32" s="2">
         <v>40626</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -1522,55 +1519,55 @@
         <v>44</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F33" s="2">
         <v>40626</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D34" s="1">
         <v>32</v>
       </c>
       <c r="E34" s="1"/>
       <c r="G34" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E35" s="1"/>
       <c r="G35" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -1578,22 +1575,22 @@
         <v>16</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F36" s="2">
         <v>40626</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1604,52 +1601,52 @@
         <v>44</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F37" s="2">
         <v>40637</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D38" s="1">
         <v>36</v>
       </c>
       <c r="E38" s="1"/>
       <c r="G38" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E39" s="1"/>
       <c r="G39" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -1660,55 +1657,55 @@
         <v>44</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F40" s="2">
         <v>40637</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D41" s="1">
         <v>39</v>
       </c>
       <c r="E41" s="1"/>
       <c r="G41" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D42" s="1">
         <v>39</v>
       </c>
       <c r="E42" s="1"/>
       <c r="G42" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -1719,30 +1716,30 @@
         <v>45</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D43" s="1">
         <v>15</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F43" s="2">
         <v>40637</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
@@ -1751,56 +1748,56 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D45" s="1">
         <v>15</v>
       </c>
       <c r="E45" s="1"/>
       <c r="G45" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D46" s="1">
         <v>15</v>
       </c>
       <c r="E46" s="1"/>
       <c r="G46" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D47" s="1">
         <v>15</v>
       </c>
       <c r="E47" s="1"/>
       <c r="G47" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -1810,102 +1807,102 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F49" s="2">
         <v>40637</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D50" s="1">
         <v>47</v>
       </c>
       <c r="E50" s="1"/>
       <c r="G50" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D51" s="1">
         <v>47</v>
       </c>
       <c r="E51" s="1"/>
       <c r="G51" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E52" s="1"/>
       <c r="G52" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F53" s="2">
         <v>40643</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -1916,55 +1913,55 @@
         <v>44</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F54" s="2">
         <v>40637</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D55" s="1">
         <v>14</v>
       </c>
       <c r="E55" s="1"/>
       <c r="G55" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E56" s="1"/>
       <c r="G56" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -1975,13 +1972,13 @@
         <v>44</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F57" s="2">
         <v>40648</v>
@@ -1995,20 +1992,20 @@
         <v>23</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D58" s="1"/>
       <c r="E58" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F58" s="2">
         <v>40648</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -2016,22 +2013,22 @@
         <v>24</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D59" s="1">
         <v>55</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F59" s="2">
         <v>40648</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -2039,20 +2036,20 @@
         <v>25</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C60" s="1"/>
       <c r="D60" s="1">
         <v>57</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F60" s="2">
         <v>40648</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -2063,19 +2060,19 @@
         <v>44</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D61" s="1">
         <v>58</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F61" s="2">
         <v>40648</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -2094,13 +2091,13 @@
         <v>44</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D63" s="1">
         <v>21</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F63" s="2">
         <v>40661</v>
@@ -2114,12 +2111,12 @@
         <v>28</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F64" s="2">
         <v>40661</v>
@@ -2134,13 +2131,13 @@
         <v>44</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F65" s="2">
         <v>40661</v>
@@ -2152,16 +2149,16 @@
         <v>30</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D66" s="1">
         <v>36</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F66" s="2">
         <v>40679</v>
@@ -2173,14 +2170,14 @@
         <v>31</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C67" s="1"/>
       <c r="D67" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F67" s="2">
         <v>40679</v>
@@ -2192,14 +2189,14 @@
         <v>32</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C68" s="1"/>
       <c r="D68" s="1">
         <v>61</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F68" s="2">
         <v>40679</v>
@@ -2211,14 +2208,14 @@
         <v>33</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C69" s="1"/>
       <c r="D69" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F69" s="2">
         <v>40679</v>
@@ -2230,14 +2227,14 @@
         <v>34</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C70" s="1"/>
       <c r="D70" s="1">
         <v>63</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F70" s="2">
         <v>40679</v>
@@ -2249,14 +2246,14 @@
         <v>35</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C71" s="1"/>
       <c r="D71" s="1">
         <v>51</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F71" s="2">
         <v>40688</v>
@@ -2268,14 +2265,14 @@
         <v>36</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C72" s="1"/>
       <c r="D72" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F72" s="2">
         <v>40688</v>
@@ -2287,14 +2284,14 @@
         <v>37</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C73" s="1"/>
       <c r="D73" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F73" s="2">
         <v>40695</v>
@@ -2309,17 +2306,17 @@
         <v>44</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D74" s="1"/>
       <c r="E74" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F74" s="2">
         <v>40618</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -2330,17 +2327,17 @@
         <v>44</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D75" s="1"/>
       <c r="E75" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F75" s="2">
         <v>40623</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -2348,20 +2345,20 @@
         <v>40</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D76" s="1"/>
       <c r="E76" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F76" s="2">
         <v>40644</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -2369,12 +2366,12 @@
         <v>41</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
       <c r="E77" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G77" s="1"/>
     </row>
@@ -2383,12 +2380,14 @@
         <v>42</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C78" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="D78" s="1"/>
       <c r="E78" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G78" s="1"/>
     </row>
@@ -2397,12 +2396,12 @@
         <v>43</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
       <c r="E79" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G79" s="1"/>
     </row>

</xml_diff>